<commit_message>
bo sung tai lieu ve db.staging
</commit_message>
<xml_diff>
--- a/docs/Control Database Design.xlsx
+++ b/docs/Control Database Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DWProject\WH_Nhom9_DongHo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AFEE7E-7426-4978-912F-F8AE3998DB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBAC095-BA96-4778-B6BE-B01D304AF7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -340,10 +340,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -369,13 +372,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>112059</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
+      <xdr:colOff>559734</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
@@ -407,8 +410,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="7153275" cy="6296025"/>
+          <a:off x="112059" y="0"/>
+          <a:ext cx="7103969" cy="6296025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -693,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="M1:Q34"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q40" sqref="Q40"/>
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +711,19 @@
     <col min="18" max="18" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
       <c r="N1" s="2" t="s">
         <v>4</v>
       </c>
@@ -716,7 +731,19 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
       <c r="N2" t="s">
         <v>0</v>
       </c>
@@ -730,7 +757,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
       <c r="M3">
         <v>1</v>
       </c>
@@ -747,7 +786,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
       <c r="M4">
         <v>2</v>
       </c>
@@ -764,7 +815,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
       <c r="M5">
         <v>3</v>
       </c>
@@ -781,7 +844,19 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
       <c r="M6">
         <v>4</v>
       </c>
@@ -798,7 +873,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
       <c r="M7">
         <v>5</v>
       </c>
@@ -815,7 +902,19 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
       <c r="M8">
         <v>6</v>
       </c>
@@ -832,7 +931,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
       <c r="M9">
         <v>7</v>
       </c>
@@ -849,7 +960,19 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
       <c r="M10">
         <v>8</v>
       </c>
@@ -866,7 +989,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
       <c r="M11">
         <v>9</v>
       </c>
@@ -883,7 +1018,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
       <c r="M12">
         <v>10</v>
       </c>
@@ -900,7 +1047,19 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
       <c r="M13">
         <v>11</v>
       </c>
@@ -917,7 +1076,19 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
       <c r="M14">
         <v>12</v>
       </c>
@@ -934,7 +1105,19 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
       <c r="M15">
         <v>13</v>
       </c>
@@ -951,10 +1134,34 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
       <c r="Q16"/>
     </row>
-    <row r="17" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
       <c r="N17" s="2" t="s">
         <v>49</v>
       </c>
@@ -962,7 +1169,19 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
       <c r="N18" t="s">
         <v>0</v>
       </c>
@@ -976,7 +1195,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
       <c r="M19">
         <v>1</v>
       </c>
@@ -993,7 +1224,19 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
       <c r="M20">
         <v>2</v>
       </c>
@@ -1010,7 +1253,19 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
       <c r="M21">
         <v>3</v>
       </c>
@@ -1027,7 +1282,19 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
       <c r="M22">
         <v>4</v>
       </c>
@@ -1044,7 +1311,19 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
       <c r="M23">
         <v>5</v>
       </c>
@@ -1061,7 +1340,19 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
       <c r="M24">
         <v>6</v>
       </c>
@@ -1078,7 +1369,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
       <c r="M25">
         <v>7</v>
       </c>
@@ -1095,7 +1398,19 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
       <c r="M26">
         <v>8</v>
       </c>
@@ -1112,7 +1427,33 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
       <c r="N28" s="2" t="s">
         <v>76</v>
       </c>
@@ -1120,7 +1461,19 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
     </row>
-    <row r="29" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
       <c r="N29" t="s">
         <v>0</v>
       </c>
@@ -1134,7 +1487,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
       <c r="M30">
         <v>1</v>
       </c>
@@ -1151,7 +1516,19 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
       <c r="M31">
         <v>2</v>
       </c>
@@ -1168,7 +1545,19 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
       <c r="M32">
         <v>3</v>
       </c>
@@ -1185,7 +1574,19 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
       <c r="M33">
         <v>4</v>
       </c>
@@ -1202,7 +1603,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="13:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M34">
         <v>5</v>
       </c>
@@ -1220,10 +1621,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="N17:Q17"/>
     <mergeCell ref="N28:Q28"/>
+    <mergeCell ref="A1:L33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
bo sung file sql, file mo hinh cau truc cay thu muc
</commit_message>
<xml_diff>
--- a/docs/Control Database Design.xlsx
+++ b/docs/Control Database Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DWProject\WH_Nhom9_DongHo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBAC095-BA96-4778-B6BE-B01D304AF7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA75900-6219-4658-ACBD-61FE0C8E8F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,9 +72,6 @@
     <t>dump_aggregate_file_path</t>
   </si>
   <si>
-    <t>copy_to_mart_script_path</t>
-  </si>
-  <si>
     <t>mart_id</t>
   </si>
   <si>
@@ -159,18 +156,9 @@
     <t>proc_load_wh_pnj</t>
   </si>
   <si>
-    <t>proc_aggregate_pnj</t>
-  </si>
-  <si>
-    <t>Đường dẫn đến file script thực hiện copy file aggregate đến máy chứa data mart</t>
-  </si>
-  <si>
     <t>D://DW/staging/load/dongho_aggregate.csv</t>
   </si>
   <si>
-    <t>D://DW/staging/load/copy_to_mart.bat</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -292,6 +280,18 @@
   </si>
   <si>
     <t>D://DW/presentation/load_to_mart.jar</t>
+  </si>
+  <si>
+    <t>aggregate_table</t>
+  </si>
+  <si>
+    <t>Tên bảng aggregate table trong warehouse</t>
+  </si>
+  <si>
+    <t>dongho_aggregate</t>
+  </si>
+  <si>
+    <t>proc_aggregate</t>
   </si>
 </sst>
 </file>
@@ -372,22 +372,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>112059</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>559734</xdr:colOff>
+      <xdr:colOff>486336</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B443BB3-6A1E-4F3E-8EBA-B83AE00B9D5B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60FF7978-EF46-4BDD-8C5D-4D4027FB9729}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -410,8 +410,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="112059" y="0"/>
-          <a:ext cx="7103969" cy="6296025"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7142630" cy="6296025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -699,7 +699,7 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,13 +774,13 @@
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q3" s="1">
         <v>1</v>
@@ -806,13 +806,13 @@
         <v>5</v>
       </c>
       <c r="O4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -835,13 +835,13 @@
         <v>6</v>
       </c>
       <c r="O5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -864,13 +864,13 @@
         <v>7</v>
       </c>
       <c r="O6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -893,13 +893,13 @@
         <v>8</v>
       </c>
       <c r="O7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -922,13 +922,13 @@
         <v>9</v>
       </c>
       <c r="O8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -951,13 +951,13 @@
         <v>10</v>
       </c>
       <c r="O9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -980,13 +980,13 @@
         <v>11</v>
       </c>
       <c r="O10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1009,13 +1009,13 @@
         <v>12</v>
       </c>
       <c r="O11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1035,16 +1035,16 @@
         <v>10</v>
       </c>
       <c r="N12" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="O12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P12" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1064,16 +1064,16 @@
         <v>11</v>
       </c>
       <c r="N13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="P13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -1093,16 +1093,16 @@
         <v>12</v>
       </c>
       <c r="N14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P14" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1122,16 +1122,16 @@
         <v>13</v>
       </c>
       <c r="N15" t="s">
+        <v>17</v>
+      </c>
+      <c r="O15" t="s">
         <v>18</v>
       </c>
-      <c r="O15" t="s">
-        <v>19</v>
-      </c>
       <c r="P15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="N17" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
@@ -1212,16 +1212,16 @@
         <v>1</v>
       </c>
       <c r="N19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="O19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -1241,16 +1241,16 @@
         <v>2</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="O20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P20" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -1270,16 +1270,16 @@
         <v>3</v>
       </c>
       <c r="N21" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="O21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P21" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -1299,16 +1299,16 @@
         <v>4</v>
       </c>
       <c r="N22" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="O22" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="P22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -1328,16 +1328,16 @@
         <v>5</v>
       </c>
       <c r="N23" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="O23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -1357,16 +1357,16 @@
         <v>6</v>
       </c>
       <c r="N24" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="O24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="P24" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -1386,16 +1386,16 @@
         <v>7</v>
       </c>
       <c r="N25" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="O25" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="P25" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -1415,16 +1415,16 @@
         <v>8</v>
       </c>
       <c r="N26" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="O26" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="P26" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -1455,7 +1455,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="N28" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
@@ -1504,16 +1504,16 @@
         <v>1</v>
       </c>
       <c r="N30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -1533,16 +1533,16 @@
         <v>2</v>
       </c>
       <c r="N31" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="O31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P31" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -1562,16 +1562,16 @@
         <v>3</v>
       </c>
       <c r="N32" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="O32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P32" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -1591,16 +1591,16 @@
         <v>4</v>
       </c>
       <c r="N33" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="O33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P33" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -1608,16 +1608,16 @@
         <v>5</v>
       </c>
       <c r="N34" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="O34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P34" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>